<commit_message>
improved mapping between ASCE and OntoGSN
</commit_message>
<xml_diff>
--- a/OntoGSN SWRL Rules.xlsx
+++ b/OntoGSN SWRL Rules.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\momcilovic\Documents\GitHub\OntoGSN_fortiss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDC4AFF-0650-4B7C-8A67-30EED2643A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB68A70-6AC2-4B84-9C03-BEA0F4F4DCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{772AD788-D383-4388-93A0-C3FA5916C595}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{772AD788-D383-4388-93A0-C3FA5916C595}"/>
   </bookViews>
   <sheets>
     <sheet name="SWRL" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SWRL!$A$1:$H$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SWRL!$A$1:$K$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -817,10 +817,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1159,17 +1162,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC5BA4E-4AEA-4D39-BDC4-88D2E47EC480}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.21875" customWidth="1"/>
+    <col min="4" max="4" width="57.21875" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="66.77734375" customWidth="1"/>
     <col min="10" max="10" width="50" customWidth="1"/>
@@ -1186,7 +1189,7 @@
       <c r="C1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>215</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1221,7 +1224,7 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
@@ -1243,7 +1246,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1253,7 +1256,7 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F3" t="s">
@@ -1266,7 +1269,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1276,7 +1279,7 @@
       <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F4" t="s">
@@ -1289,7 +1292,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1299,7 +1302,7 @@
       <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F5" t="s">
@@ -1312,7 +1315,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1322,7 +1325,7 @@
       <c r="C6" t="s">
         <v>86</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F6" t="s">
@@ -1335,7 +1338,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1345,7 +1348,7 @@
       <c r="C7" t="s">
         <v>94</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F7" t="s">
@@ -1358,7 +1361,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1368,7 +1371,7 @@
       <c r="C8" t="s">
         <v>96</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>97</v>
       </c>
       <c r="F8" t="s">
@@ -1391,7 +1394,7 @@
       <c r="C9" t="s">
         <v>98</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>99</v>
       </c>
       <c r="F9" t="s">
@@ -1407,7 +1410,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1417,7 +1420,7 @@
       <c r="C10" t="s">
         <v>100</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>101</v>
       </c>
       <c r="F10" t="s">
@@ -1440,7 +1443,7 @@
       <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F11" t="s">
@@ -1463,7 +1466,7 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F12" t="s">
@@ -1479,7 +1482,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1489,7 +1492,7 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F13" t="s">
@@ -1502,7 +1505,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1512,7 +1515,7 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
@@ -1525,7 +1528,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1535,7 +1538,7 @@
       <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F15" t="s">
@@ -1548,7 +1551,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1558,7 +1561,7 @@
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
@@ -1571,7 +1574,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1581,7 +1584,7 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F17" t="s">
@@ -1594,7 +1597,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1604,7 +1607,7 @@
       <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F18" t="s">
@@ -1617,7 +1620,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1627,7 +1630,7 @@
       <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F19" t="s">
@@ -1640,7 +1643,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1650,7 +1653,7 @@
       <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F20" t="s">
@@ -1663,7 +1666,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1673,7 +1676,7 @@
       <c r="C21" t="s">
         <v>24</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F21" t="s">
@@ -1686,7 +1689,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1696,7 +1699,7 @@
       <c r="C22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F22" t="s">
@@ -1709,7 +1712,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1719,7 +1722,7 @@
       <c r="C23" t="s">
         <v>28</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F23" t="s">
@@ -1732,7 +1735,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1742,7 +1745,7 @@
       <c r="C24" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F24" t="s">
@@ -1755,7 +1758,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1765,7 +1768,7 @@
       <c r="C25" t="s">
         <v>32</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F25" t="s">
@@ -1778,7 +1781,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1788,7 +1791,7 @@
       <c r="C26" t="s">
         <v>34</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F26" t="s">
@@ -1801,7 +1804,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1811,7 +1814,7 @@
       <c r="C27" t="s">
         <v>36</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F27" t="s">
@@ -1824,7 +1827,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1834,7 +1837,7 @@
       <c r="C28" t="s">
         <v>38</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F28" t="s">
@@ -1847,7 +1850,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1857,7 +1860,7 @@
       <c r="C29" t="s">
         <v>40</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>41</v>
       </c>
       <c r="F29" t="s">
@@ -1870,7 +1873,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1880,7 +1883,7 @@
       <c r="C30" t="s">
         <v>44</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>45</v>
       </c>
       <c r="F30" t="s">
@@ -1893,7 +1896,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1903,7 +1906,7 @@
       <c r="C31" t="s">
         <v>46</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F31" t="s">
@@ -1916,7 +1919,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>32</v>
       </c>
@@ -1926,7 +1929,7 @@
       <c r="C32" t="s">
         <v>48</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F32" t="s">
@@ -1939,7 +1942,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1949,7 +1952,7 @@
       <c r="C33" t="s">
         <v>50</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F33" t="s">
@@ -1962,7 +1965,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>34</v>
       </c>
@@ -1972,7 +1975,7 @@
       <c r="C34" t="s">
         <v>52</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F34" t="s">
@@ -1985,7 +1988,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>35</v>
       </c>
@@ -1995,7 +1998,7 @@
       <c r="C35" t="s">
         <v>54</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F35" t="s">
@@ -2008,7 +2011,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2018,7 +2021,7 @@
       <c r="C36" t="s">
         <v>56</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F36" t="s">
@@ -2031,7 +2034,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>37</v>
       </c>
@@ -2041,7 +2044,7 @@
       <c r="C37" t="s">
         <v>58</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F37" t="s">
@@ -2064,7 +2067,7 @@
       <c r="C38" t="s">
         <v>60</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F38" t="s">
@@ -2077,7 +2080,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>39</v>
       </c>
@@ -2087,7 +2090,7 @@
       <c r="C39" t="s">
         <v>62</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F39" t="s">
@@ -2100,7 +2103,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>40</v>
       </c>
@@ -2110,7 +2113,7 @@
       <c r="C40" t="s">
         <v>66</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>67</v>
       </c>
       <c r="F40" t="s">
@@ -2123,7 +2126,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>41</v>
       </c>
@@ -2133,7 +2136,7 @@
       <c r="C41" t="s">
         <v>68</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>69</v>
       </c>
       <c r="F41" t="s">
@@ -2146,7 +2149,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>42</v>
       </c>
@@ -2156,7 +2159,7 @@
       <c r="C42" t="s">
         <v>70</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F42" t="s">
@@ -2169,7 +2172,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>43</v>
       </c>
@@ -2179,7 +2182,7 @@
       <c r="C43" t="s">
         <v>72</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F43" t="s">
@@ -2192,7 +2195,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>44</v>
       </c>
@@ -2202,7 +2205,7 @@
       <c r="C44" t="s">
         <v>74</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F44" t="s">
@@ -2215,7 +2218,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2225,7 +2228,7 @@
       <c r="C45" t="s">
         <v>76</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>77</v>
       </c>
       <c r="F45" t="s">
@@ -2248,7 +2251,7 @@
       <c r="C46" t="s">
         <v>78</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F46" t="s">
@@ -2271,7 +2274,7 @@
       <c r="C47" t="s">
         <v>80</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>81</v>
       </c>
       <c r="F47" t="s">
@@ -2294,7 +2297,7 @@
       <c r="C48" t="s">
         <v>82</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F48" t="s">
@@ -2307,7 +2310,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2317,7 +2320,7 @@
       <c r="C49" t="s">
         <v>84</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F49" t="s">
@@ -2330,7 +2333,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2340,7 +2343,7 @@
       <c r="C50" t="s">
         <v>88</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F50" t="s">
@@ -2353,7 +2356,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2363,7 +2366,7 @@
       <c r="C51" t="s">
         <v>90</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>91</v>
       </c>
       <c r="F51" t="s">
@@ -2386,7 +2389,7 @@
       <c r="C52" t="s">
         <v>92</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F52" t="s">
@@ -2400,7 +2403,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H52" xr:uid="{6EC5BA4E-4AEA-4D39-BDC4-88D2E47EC480}"/>
+  <autoFilter ref="A1:K52" xr:uid="{6EC5BA4E-4AEA-4D39-BDC4-88D2E47EC480}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved swrl documentation & diagram
</commit_message>
<xml_diff>
--- a/OntoGSN SWRL Rules.xlsx
+++ b/OntoGSN SWRL Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\momcilovic\Documents\GitHub\OntoGSN_fortiss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB68A70-6AC2-4B84-9C03-BEA0F4F4DCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749691D9-B220-425B-B156-2B55D011BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{772AD788-D383-4388-93A0-C3FA5916C595}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{772AD788-D383-4388-93A0-C3FA5916C595}"/>
   </bookViews>
   <sheets>
     <sheet name="SWRL" sheetId="1" r:id="rId1"/>
@@ -1163,7 +1163,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
improved the rule representation in SPARQL
</commit_message>
<xml_diff>
--- a/OntoGSN SWRL Rules.xlsx
+++ b/OntoGSN SWRL Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\momcilovic\Documents\GitHub\OntoGSN_fortiss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749691D9-B220-425B-B156-2B55D011BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CF07F8-1009-47E4-A5E9-384733910021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{772AD788-D383-4388-93A0-C3FA5916C595}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{772AD788-D383-4388-93A0-C3FA5916C595}"/>
   </bookViews>
   <sheets>
     <sheet name="SWRL" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="266">
   <si>
     <t>S1</t>
   </si>
@@ -773,6 +773,668 @@
      gsn:true ?tA .
   FILTER(xsd:boolean(?tA) = false)
   ?B gsn:supportedBy* ?A .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?R rdf:subject ?A ;
+     rdf:object  ?B .
+  ?A gsn:inContextOf ?B .
+  BIND(?R AS ?s)
+  BIND(gsn:relationshipType AS ?p)
+  BIND("contextual" AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?B a gsn:Solution .
+  ?A gsn:supportedBy ?B .
+  ?R rdf:subject ?A ;
+     rdf:object  ?B .
+  BIND(?R AS ?s)
+  BIND(gsn:relationshipType AS ?p)
+  BIND("evidential" AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?B a gsn:Strategy .
+  ?A gsn:supportedBy ?B .
+  ?R rdf:subject ?A ;
+     rdf:object  ?B .
+  BIND(?R AS ?s)
+  BIND(gsn:relationshipType AS ?p)
+  BIND("inferential" AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?B a gsn:Goal .
+  ?A gsn:supportedBy ?B .
+  ?R rdf:subject ?A ;
+     rdf:object  ?B .
+  BIND(?R AS ?s)
+  BIND(gsn:relationshipType AS ?p)
+  BIND("inferential" AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A a gsn:Goal .
+  ?X gsn:supportedBy ?A .
+  ?A gsn:supportedBy ?B .
+  BIND(?A AS ?s)
+  BIND(gsn:top AS ?p)
+  BIND(false AS ?o)   # xsd:boolean false
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?R1 rdf:subject ?A ;
+      rdf:object  ?B ;
+      rdf:predicate ?P .
+  ?R2 rdf:subject ?B ;
+      rdf:object  ?C ;
+      rdf:predicate ?P .
+  ?R3 rdf:subject ?C ;
+      rdf:object  ?A ;
+      rdf:predicate ?P .
+  FILTER(?R1 != ?R2 &amp;&amp; ?R1 != ?R3 &amp;&amp; ?R2 != ?R3)
+  # Report all three R1, R2, R3 needing valid=false:
+  {
+    BIND(?R1 AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+  UNION
+  {
+    BIND(?R2 AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+  UNION
+  {
+    BIND(?R3 AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?C gsn:true true ;
+     gsn:supportedBy ?A, ?B .
+  ?A a gsn:Goal ;
+     gsn:true true .
+  ?B a gsn:Goal ;
+     gsn:true true .
+  FILTER(?A != ?B)
+  BIND(?C AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A a gsn:Solution ;
+     gsn:true true .
+  ?B gsn:supportedBy ?A .
+  BIND(?B AS ?s)
+  BIND(gsn:true AS ?p)
+  BIND(true AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?B gsn:valid false .
+  ?A gsn:valid true .
+  ?C gsn:supportedBy ?B, ?A .
+  FILTER(?A != ?B)
+  BIND(?C AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A a gsn:Solution ;
+     gsn:true true .
+  ?B a gsn:Solution ;
+     gsn:true false .
+  ?C gsn:supportedBy ?A, ?B .
+  FILTER(?A != ?B)
+  BIND(?C AS ?s)
+  BIND(gsn:true AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?R a gsn:Relationship ;
+     gsn:true false ;
+     rdf:subject ?A ;
+     rdf:object  ?B .
+  ?A gsn:inContextOf ?B .
+  BIND(?A AS ?s)
+  BIND(gsn:true AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A a gsn:Assumption ;
+     gsn:true false .
+  ?B gsn:inContextOf ?A .
+  BIND(?B AS ?s)
+  BIND(gsn:true AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A a gsn:Assumption .
+  ?C a gsn:Goal .
+  ?B gsn:supportedBy ?C ;
+     gsn:inContextOf  ?A .
+  BIND(?C AS ?s)
+  BIND(gsn:inContextOf AS ?p)
+  BIND(?A AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A gsn:supportedBy ?B .
+  # Example: deterministically generate a relationship IRI
+  BIND(IRI(CONCAT("https://w3id.org/OntoGSN/rel/",
+                  ENCODE_FOR_URI(STR(?A)), "_",
+                  ENCODE_FOR_URI(STR(?B)))) AS ?R)
+  {
+    BIND(?R AS ?s)
+    BIND(rdf:subject AS ?p)
+    BIND(?A AS ?o)
+  }
+  UNION
+  {
+    BIND(?R AS ?s)
+    BIND(rdf:object AS ?p)
+    BIND(?B AS ?o)
+  }
+  UNION
+  {
+    BIND(?R AS ?s)
+    BIND(rdf:type AS ?p)
+    BIND(gsn:Relationship AS ?o)
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A gsn:inContextOf ?B .
+  BIND(IRI(CONCAT("https://w3id.org/OntoGSN/rel/",
+                  ENCODE_FOR_URI(STR(?A)), "_ctx_",
+                  ENCODE_FOR_URI(STR(?B)))) AS ?R)
+  {
+    BIND(?R AS ?s)
+    BIND(rdf:subject AS ?p)
+    BIND(?A AS ?o)
+  }
+  UNION
+  {
+    BIND(?R AS ?s)
+    BIND(rdf:object AS ?p)
+    BIND(?B AS ?o)
+  }
+  UNION
+  {
+    BIND(?R AS ?s)
+    BIND(rdf:type AS ?p)
+    BIND(gsn:Relationship AS ?o)
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?C a gsn:Pattern .
+  ?B gsn:instantiationOf ?C .
+  ?A gsn:final true ;
+     gsn:contains ?B, ?C .
+  BIND(?A AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A a gsn:Template ;
+     gsn:published true .
+  ?R gsn:undeveloped true ;
+     rdf:subject    ?A .
+  {
+    BIND(?A AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+  UNION
+  {
+    BIND(?R AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf:  &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A a gsn:Template ;
+     gsn:published true ;
+     gsn:contains  ?B .
+  ?R gsn:undeveloped true ;
+     rdf:subject    ?B .
+  {
+    BIND(?A AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+  UNION
+  {
+    BIND(?R AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M a gsn:Module ;
+     gsn:contains ?A .
+  ?N a gsn:Module ;
+     gsn:contains ?B .
+  ?A gsn:supportedBy ?B .
+  FILTER(?M != ?N)
+  BIND(?B AS ?s)
+  BIND(gsn:away AS ?p)
+  BIND(true AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:  &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M a gsn:Module ;
+     gsn:contains ?A .
+  ?N a gsn:Module ;
+     gsn:contains ?B .
+  ?A gsn:inContextOf ?B .
+  FILTER(?M != ?N)
+  BIND(?B AS ?s)
+  BIND(gsn:away AS ?p)
+  BIND(true AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn:    &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX schema: &lt;http://schema.org/&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M a gsn:Module ;
+     gsn:contains ?A, ?B .
+  ?A schema:identifier ?id .
+  ?B schema:identifier ?id .
+  FILTER(?A != ?B)
+  {
+    BIND(?A AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+  UNION
+  {
+    BIND(?B AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M1 a gsn:Module .
+  ?M2 a gsn:Module ;
+      gsn:contains ?A ;
+      gsn:contract true .
+  ?A gsn:supportedBy ?M1 .
+  ?R rdf:subject ?A ;
+     rdf:object  ?M1 .
+  BIND(?R AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M1 a gsn:Module .
+  ?M2 a gsn:Module ;
+      gsn:contains ?A ;
+      gsn:contract true .
+  ?A gsn:inContextOf ?M1 .
+  ?R rdf:subject ?A ;
+     rdf:object  ?M1 .
+  BIND(?R AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M a gsn:Module ;
+     gsn:contains ?A ;
+     gsn:contract true .
+  ?A gsn:toBeSupportedByContract true .
+  BIND(?A AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?G1 a gsn:Goal ;
+      gsn:supportedBy ?G2 ;
+      gsn:away true .
+  ?R rdf:subject ?G1 ;
+     rdf:object  ?G2 .
+  ?M1 a gsn:Module ;
+      gsn:contains ?G1 .
+  ?M2 a gsn:Module ;
+      gsn:contains ?G2 .
+  BIND(?R AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A gsn:away true ;
+     gsn:toBeSupportedByContract true ;
+     gsn:supportedBy ?B .
+  ?M1 a gsn:Module ;
+      gsn:contains ?A .
+  ?M2 a gsn:Module ;
+      gsn:contains ?B .
+  FILTER(?M1 != ?M2)
+  BIND(?M2 AS ?s)
+  BIND(gsn:contract AS ?p)
+  BIND(true AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+PREFIX rdf: &lt;http://www.w3.org/1999/02/22-rdf-syntax-ns#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M a gsn:Module ;
+     gsn:contains ?A, ?B .
+  ?A gsn:toBeSupportedByContract true ;
+     gsn:supportedBy ?B .
+  ?R rdf:subject ?A ;
+     rdf:object  ?B .
+  BIND(?R AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?G1 a gsn:Goal ;
+      gsn:inContextOf ?C1 ;
+      gsn:supportedBy ?G2 .
+  ?G2 a gsn:Goal ;
+      gsn:inContextOf ?C2 ;
+      gsn:away true .
+  ?C2 a gsn:Context .
+  BIND(?C1 AS ?s)
+  BIND(gsn:consistentWith AS ?p)
+  BIND(?C2 AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M1 a gsn:Module ;
+      gsn:contains ?J .
+  ?M2 a gsn:Module ;
+      gsn:contains ?G .
+  FILTER(?M1 != ?M2)
+  ?J a gsn:Justification ;
+     gsn:substitutedBy ?G .
+  ?E gsn:inContextOf ?J .
+  BIND(?J AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>PREFIX gsn: &lt;https://w3id.org/OntoGSN/ontology#&gt;
+SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M1 a gsn:Module ;
+      gsn:contains ?E1 .
+  ?M2 a gsn:Module ;
+      gsn:contains ?E2 .
+  FILTER(?M1 != ?M2)
+  ?E1 gsn:supportedBy ?E2 .
+  BIND(?M1 AS ?s)
+  BIND(gsn:supportedBy AS ?p)
+  BIND(?M2 AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M1 a gsn:Module ;
+      gsn:contains ?E1 .
+  ?M2 a gsn:Module ;
+      gsn:contains ?E2 .
+  FILTER(?M1 != ?M2)
+  ?E1 gsn:inContextOf ?E2 .
+  BIND(?M1 AS ?s)
+  BIND(gsn:inContextOf AS ?p)
+  BIND(?M2 AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M1 a gsn:Module ;
+      gsn:contains ?E1 .
+  ?M2 a gsn:Module .
+  ?E1 gsn:supportedBy ?M2 .
+  FILTER(?M1 != ?M2)
+  BIND(?M1 AS ?s)
+  BIND(gsn:supportedBy AS ?p)
+  BIND(?M2 AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?M1 a gsn:Module ;
+      gsn:supportedBy ?M2 .
+  ?M2 a gsn:Module ;
+      gsn:supportedBy ?M3 .
+  ?M3 a gsn:Module ;
+      gsn:supportedBy ?M1 .
+  FILTER(?M1 != ?M2 &amp;&amp; ?M1 != ?M3 &amp;&amp; ?M2 != ?M3)
+  {
+    BIND(?M1 AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+  UNION
+  {
+    BIND(?M2 AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+  UNION
+  {
+    BIND(?M3 AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?G a gsn:Goal ;
+     gsn:public true ;
+     gsn:inContextOf ?C .
+  BIND(?C AS ?s)
+  BIND(gsn:public AS ?p)
+  BIND(true AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?C gsn:contract true ;
+     gsn:contains ?E .
+  ?E gsn:public true .
+  BIND(?E AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A schema:identifier ?id .
+  ?B schema:identifier ?id .
+  FILTER(?A != ?B)
+  {
+    BIND(?A AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+  UNION
+  {
+    BIND(?B AS ?s)
+    BIND(gsn:valid AS ?p)
+    BIND(false AS ?o)
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?S a gsn:Solution ;
+     gsn:valid true ;
+     gsn:challenges ?E .
+  BIND(?E AS ?s)
+  BIND(gsn:defeated AS ?p)
+  BIND(true AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?E gsn:defeated true .
+  BIND(?E AS ?s)
+  BIND(gsn:valid AS ?p)
+  BIND(false AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?G a gsn:Goal ;
+     gsn:true true ;
+     gsn:challenges ?E .
+  BIND(?E AS ?s)
+  BIND(gsn:inDoubt AS ?p)
+  BIND(true AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?G a gsn:Goal ;
+     gsn:undeveloped false ;
+     gsn:challenges ?E .
+  ?E gsn:inDoubt true .
+  BIND(?E AS ?s)
+  BIND(gsn:defeated AS ?p)
+  BIND(true AS ?o)
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?s ?p ?o
+WHERE {
+  ?A gsn:challenges ?B .
+  BIND(?A AS ?s)
+  BIND(rdf:type AS ?p)
+  BIND(gsn:Defeater AS ?o)
 }</t>
   </si>
 </sst>
@@ -1162,18 +1824,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC5BA4E-4AEA-4D39-BDC4-88D2E47EC480}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" customWidth="1"/>
-    <col min="7" max="7" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="34.21875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="66.77734375" customWidth="1"/>
     <col min="10" max="10" width="50" customWidth="1"/>
     <col min="11" max="11" width="58.109375" customWidth="1"/>
@@ -1246,7 +1909,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1268,8 +1931,11 @@
       <c r="H3" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I3" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1291,8 +1957,11 @@
       <c r="H4" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I4" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1314,8 +1983,11 @@
       <c r="H5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I5" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1337,8 +2009,11 @@
       <c r="H6" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I6" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1360,8 +2035,11 @@
       <c r="H7" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I7" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1382,6 +2060,9 @@
       </c>
       <c r="H8" t="s">
         <v>209</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="345.6" x14ac:dyDescent="0.3">
@@ -1410,7 +2091,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1432,8 +2113,11 @@
       <c r="H10" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1454,6 +2138,9 @@
       </c>
       <c r="H11" t="s">
         <v>209</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="144" x14ac:dyDescent="0.3">
@@ -1482,7 +2169,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="216" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1504,8 +2191,11 @@
       <c r="H13" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I13" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1527,8 +2217,11 @@
       <c r="H14" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I14" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1550,8 +2243,11 @@
       <c r="H15" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I15" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1573,8 +2269,11 @@
       <c r="H16" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I16" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1596,8 +2295,11 @@
       <c r="H17" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I17" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1619,8 +2321,11 @@
       <c r="H18" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I18" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1642,8 +2347,11 @@
       <c r="H19" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I19" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1665,8 +2373,11 @@
       <c r="H20" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I20" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1688,8 +2399,11 @@
       <c r="H21" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I21" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1711,8 +2425,11 @@
       <c r="H22" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I22" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1734,8 +2451,11 @@
       <c r="H23" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I23" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1757,8 +2477,11 @@
       <c r="H24" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I24" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="360" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1780,8 +2503,11 @@
       <c r="H25" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I25" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1803,8 +2529,11 @@
       <c r="H26" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I26" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1826,8 +2555,11 @@
       <c r="H27" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I27" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1849,8 +2581,11 @@
       <c r="H28" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I28" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1872,8 +2607,11 @@
       <c r="H29" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I29" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="288" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1895,8 +2633,11 @@
       <c r="H30" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I30" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1918,8 +2659,11 @@
       <c r="H31" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I31" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>32</v>
       </c>
@@ -1941,8 +2685,11 @@
       <c r="H32" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I32" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1964,8 +2711,11 @@
       <c r="H33" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I33" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>34</v>
       </c>
@@ -1987,8 +2737,11 @@
       <c r="H34" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I34" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2010,8 +2763,11 @@
       <c r="H35" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I35" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2033,8 +2789,11 @@
       <c r="H36" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="I36" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>37</v>
       </c>
@@ -2056,8 +2815,11 @@
       <c r="H37" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>38</v>
       </c>
@@ -2079,8 +2841,11 @@
       <c r="H38" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I38" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>39</v>
       </c>
@@ -2102,8 +2867,11 @@
       <c r="H39" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I39" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>40</v>
       </c>
@@ -2126,7 +2894,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>41</v>
       </c>
@@ -2148,8 +2916,11 @@
       <c r="H41" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="I41" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>42</v>
       </c>
@@ -2172,7 +2943,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>43</v>
       </c>
@@ -2195,7 +2966,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>44</v>
       </c>
@@ -2218,7 +2989,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2241,7 +3012,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2263,8 +3034,11 @@
       <c r="H46" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2286,8 +3060,11 @@
       <c r="H47" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>48</v>
       </c>
@@ -2309,8 +3086,11 @@
       <c r="H48" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I48" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2332,8 +3112,11 @@
       <c r="H49" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I49" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2356,7 +3139,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2379,7 +3162,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2400,6 +3183,9 @@
       </c>
       <c r="H52" t="s">
         <v>210</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>